<commit_message>
change properties name, add some tests
</commit_message>
<xml_diff>
--- a/datamanagement-service/src/main/resources/schuelerliste.xlsx
+++ b/datamanagement-service/src/main/resources/schuelerliste.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aneub\IdeaProjects\BWV-BOT\datamanagement-service\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED543B0B-4BF0-4561-953B-5BFE89891F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D122AFF0-B9CE-45F3-B79E-F913DA828025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="3552" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="student" sheetId="1" r:id="rId1"/>
@@ -1279,7 +1279,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2133,11 +2133,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2150,10 +2150,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -2161,10 +2161,10 @@
         <v>268</v>
       </c>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -2172,10 +2172,10 @@
         <v>269</v>
       </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -2183,10 +2183,10 @@
         <v>267</v>
       </c>
       <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -2194,10 +2194,10 @@
         <v>270</v>
       </c>
       <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
         <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -2205,10 +2205,10 @@
         <v>271</v>
       </c>
       <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
         <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -2216,10 +2216,10 @@
         <v>272</v>
       </c>
       <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
         <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -2227,10 +2227,10 @@
         <v>273</v>
       </c>
       <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
         <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -2238,10 +2238,10 @@
         <v>274</v>
       </c>
       <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
         <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -2249,10 +2249,10 @@
         <v>275</v>
       </c>
       <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
         <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -2260,10 +2260,10 @@
         <v>276</v>
       </c>
       <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
         <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -2271,10 +2271,10 @@
         <v>277</v>
       </c>
       <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
         <v>23</v>
-      </c>
-      <c r="C12" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -2282,10 +2282,10 @@
         <v>278</v>
       </c>
       <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
         <v>25</v>
-      </c>
-      <c r="C13" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -2293,10 +2293,10 @@
         <v>279</v>
       </c>
       <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
         <v>27</v>
-      </c>
-      <c r="C14" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -2304,10 +2304,10 @@
         <v>280</v>
       </c>
       <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
         <v>29</v>
-      </c>
-      <c r="C15" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -2315,10 +2315,10 @@
         <v>281</v>
       </c>
       <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
         <v>31</v>
-      </c>
-      <c r="C16" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -2326,10 +2326,10 @@
         <v>282</v>
       </c>
       <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
         <v>31</v>
-      </c>
-      <c r="C17" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -2337,10 +2337,10 @@
         <v>283</v>
       </c>
       <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
         <v>34</v>
-      </c>
-      <c r="C18" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -2348,10 +2348,10 @@
         <v>284</v>
       </c>
       <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" t="s">
         <v>36</v>
-      </c>
-      <c r="C19" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -2359,10 +2359,10 @@
         <v>285</v>
       </c>
       <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
         <v>38</v>
-      </c>
-      <c r="C20" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -2370,10 +2370,10 @@
         <v>286</v>
       </c>
       <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
         <v>40</v>
-      </c>
-      <c r="C21" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -2381,10 +2381,10 @@
         <v>287</v>
       </c>
       <c r="B22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" t="s">
         <v>41</v>
-      </c>
-      <c r="C22" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -2392,10 +2392,10 @@
         <v>288</v>
       </c>
       <c r="B23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" t="s">
         <v>43</v>
-      </c>
-      <c r="C23" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -2403,10 +2403,10 @@
         <v>289</v>
       </c>
       <c r="B24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" t="s">
         <v>45</v>
-      </c>
-      <c r="C24" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -2414,10 +2414,10 @@
         <v>290</v>
       </c>
       <c r="B25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" t="s">
         <v>47</v>
-      </c>
-      <c r="C25" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -2425,10 +2425,10 @@
         <v>291</v>
       </c>
       <c r="B26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" t="s">
         <v>48</v>
-      </c>
-      <c r="C26" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -2436,10 +2436,10 @@
         <v>292</v>
       </c>
       <c r="B27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" t="s">
         <v>50</v>
-      </c>
-      <c r="C27" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -2447,10 +2447,10 @@
         <v>293</v>
       </c>
       <c r="B28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" t="s">
         <v>31</v>
-      </c>
-      <c r="C28" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -2458,10 +2458,10 @@
         <v>294</v>
       </c>
       <c r="B29" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" t="s">
         <v>52</v>
-      </c>
-      <c r="C29" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -2469,10 +2469,10 @@
         <v>295</v>
       </c>
       <c r="B30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" t="s">
         <v>54</v>
-      </c>
-      <c r="C30" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -2480,10 +2480,10 @@
         <v>296</v>
       </c>
       <c r="B31" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" t="s">
         <v>56</v>
-      </c>
-      <c r="C31" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -2491,10 +2491,10 @@
         <v>297</v>
       </c>
       <c r="B32" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" t="s">
         <v>58</v>
-      </c>
-      <c r="C32" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -2502,10 +2502,10 @@
         <v>298</v>
       </c>
       <c r="B33" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" t="s">
         <v>60</v>
-      </c>
-      <c r="C33" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -2513,10 +2513,10 @@
         <v>299</v>
       </c>
       <c r="B34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" t="s">
         <v>62</v>
-      </c>
-      <c r="C34" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -2524,10 +2524,10 @@
         <v>300</v>
       </c>
       <c r="B35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" t="s">
         <v>63</v>
-      </c>
-      <c r="C35" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -2535,10 +2535,10 @@
         <v>291</v>
       </c>
       <c r="B36" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" t="s">
         <v>65</v>
-      </c>
-      <c r="C36" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -2546,10 +2546,10 @@
         <v>301</v>
       </c>
       <c r="B37" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" t="s">
         <v>65</v>
-      </c>
-      <c r="C37" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -2557,10 +2557,10 @@
         <v>302</v>
       </c>
       <c r="B38" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" t="s">
         <v>68</v>
-      </c>
-      <c r="C38" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -2568,10 +2568,10 @@
         <v>303</v>
       </c>
       <c r="B39" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" t="s">
         <v>56</v>
-      </c>
-      <c r="C39" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -2579,10 +2579,10 @@
         <v>304</v>
       </c>
       <c r="B40" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" t="s">
         <v>71</v>
-      </c>
-      <c r="C40" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -2590,10 +2590,10 @@
         <v>305</v>
       </c>
       <c r="B41" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" t="s">
         <v>73</v>
-      </c>
-      <c r="C41" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -2601,10 +2601,10 @@
         <v>306</v>
       </c>
       <c r="B42" t="s">
+        <v>76</v>
+      </c>
+      <c r="C42" t="s">
         <v>75</v>
-      </c>
-      <c r="C42" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -2612,10 +2612,10 @@
         <v>307</v>
       </c>
       <c r="B43" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" t="s">
         <v>77</v>
-      </c>
-      <c r="C43" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -2623,10 +2623,10 @@
         <v>308</v>
       </c>
       <c r="B44" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" t="s">
         <v>79</v>
-      </c>
-      <c r="C44" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -2634,10 +2634,10 @@
         <v>309</v>
       </c>
       <c r="B45" t="s">
+        <v>82</v>
+      </c>
+      <c r="C45" t="s">
         <v>81</v>
-      </c>
-      <c r="C45" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -2645,10 +2645,10 @@
         <v>310</v>
       </c>
       <c r="B46" t="s">
+        <v>83</v>
+      </c>
+      <c r="C46" t="s">
         <v>76</v>
-      </c>
-      <c r="C46" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -2656,10 +2656,10 @@
         <v>311</v>
       </c>
       <c r="B47" t="s">
+        <v>84</v>
+      </c>
+      <c r="C47" t="s">
         <v>52</v>
-      </c>
-      <c r="C47" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -2667,10 +2667,10 @@
         <v>312</v>
       </c>
       <c r="B48" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48" t="s">
         <v>85</v>
-      </c>
-      <c r="C48" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -2678,10 +2678,10 @@
         <v>313</v>
       </c>
       <c r="B49" t="s">
+        <v>39</v>
+      </c>
+      <c r="C49" t="s">
         <v>86</v>
-      </c>
-      <c r="C49" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -2689,10 +2689,10 @@
         <v>314</v>
       </c>
       <c r="B50" t="s">
+        <v>30</v>
+      </c>
+      <c r="C50" t="s">
         <v>17</v>
-      </c>
-      <c r="C50" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
@@ -2700,10 +2700,10 @@
         <v>315</v>
       </c>
       <c r="B51" t="s">
+        <v>88</v>
+      </c>
+      <c r="C51" t="s">
         <v>87</v>
-      </c>
-      <c r="C51" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
@@ -2711,10 +2711,10 @@
         <v>285</v>
       </c>
       <c r="B52" t="s">
+        <v>37</v>
+      </c>
+      <c r="C52" t="s">
         <v>89</v>
-      </c>
-      <c r="C52" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
@@ -2722,10 +2722,10 @@
         <v>316</v>
       </c>
       <c r="B53" t="s">
+        <v>91</v>
+      </c>
+      <c r="C53" t="s">
         <v>90</v>
-      </c>
-      <c r="C53" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
@@ -2733,10 +2733,10 @@
         <v>317</v>
       </c>
       <c r="B54" t="s">
+        <v>93</v>
+      </c>
+      <c r="C54" t="s">
         <v>92</v>
-      </c>
-      <c r="C54" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
@@ -2744,10 +2744,10 @@
         <v>318</v>
       </c>
       <c r="B55" t="s">
+        <v>76</v>
+      </c>
+      <c r="C55" t="s">
         <v>94</v>
-      </c>
-      <c r="C55" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
@@ -2755,10 +2755,10 @@
         <v>319</v>
       </c>
       <c r="B56" t="s">
+        <v>95</v>
+      </c>
+      <c r="C56" t="s">
         <v>75</v>
-      </c>
-      <c r="C56" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
@@ -2766,10 +2766,10 @@
         <v>320</v>
       </c>
       <c r="B57" t="s">
+        <v>97</v>
+      </c>
+      <c r="C57" t="s">
         <v>96</v>
-      </c>
-      <c r="C57" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
@@ -2777,10 +2777,10 @@
         <v>321</v>
       </c>
       <c r="B58" t="s">
+        <v>99</v>
+      </c>
+      <c r="C58" t="s">
         <v>98</v>
-      </c>
-      <c r="C58" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
@@ -2788,10 +2788,10 @@
         <v>322</v>
       </c>
       <c r="B59" t="s">
+        <v>57</v>
+      </c>
+      <c r="C59" t="s">
         <v>100</v>
-      </c>
-      <c r="C59" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
@@ -2799,10 +2799,10 @@
         <v>323</v>
       </c>
       <c r="B60" t="s">
+        <v>33</v>
+      </c>
+      <c r="C60" t="s">
         <v>101</v>
-      </c>
-      <c r="C60" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
@@ -2810,10 +2810,10 @@
         <v>324</v>
       </c>
       <c r="B61" t="s">
+        <v>103</v>
+      </c>
+      <c r="C61" t="s">
         <v>102</v>
-      </c>
-      <c r="C61" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
@@ -2821,10 +2821,10 @@
         <v>325</v>
       </c>
       <c r="B62" t="s">
+        <v>104</v>
+      </c>
+      <c r="C62" t="s">
         <v>101</v>
-      </c>
-      <c r="C62" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
@@ -2832,10 +2832,10 @@
         <v>326</v>
       </c>
       <c r="B63" t="s">
+        <v>88</v>
+      </c>
+      <c r="C63" t="s">
         <v>105</v>
-      </c>
-      <c r="C63" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
@@ -2843,10 +2843,10 @@
         <v>327</v>
       </c>
       <c r="B64" t="s">
+        <v>106</v>
+      </c>
+      <c r="C64" t="s">
         <v>101</v>
-      </c>
-      <c r="C64" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
@@ -2854,10 +2854,10 @@
         <v>328</v>
       </c>
       <c r="B65" t="s">
+        <v>108</v>
+      </c>
+      <c r="C65" t="s">
         <v>107</v>
-      </c>
-      <c r="C65" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
@@ -2865,10 +2865,10 @@
         <v>329</v>
       </c>
       <c r="B66" t="s">
+        <v>109</v>
+      </c>
+      <c r="C66" t="s">
         <v>17</v>
-      </c>
-      <c r="C66" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
@@ -2876,10 +2876,10 @@
         <v>330</v>
       </c>
       <c r="B67" t="s">
+        <v>111</v>
+      </c>
+      <c r="C67" t="s">
         <v>110</v>
-      </c>
-      <c r="C67" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
@@ -2887,10 +2887,10 @@
         <v>331</v>
       </c>
       <c r="B68" t="s">
+        <v>112</v>
+      </c>
+      <c r="C68" t="s">
         <v>27</v>
-      </c>
-      <c r="C68" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
@@ -2898,10 +2898,10 @@
         <v>332</v>
       </c>
       <c r="B69" t="s">
+        <v>114</v>
+      </c>
+      <c r="C69" t="s">
         <v>113</v>
-      </c>
-      <c r="C69" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
@@ -2909,10 +2909,10 @@
         <v>333</v>
       </c>
       <c r="B70" t="s">
+        <v>115</v>
+      </c>
+      <c r="C70" t="s">
         <v>31</v>
-      </c>
-      <c r="C70" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
@@ -2920,10 +2920,10 @@
         <v>334</v>
       </c>
       <c r="B71" t="s">
+        <v>99</v>
+      </c>
+      <c r="C71" t="s">
         <v>116</v>
-      </c>
-      <c r="C71" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
@@ -2931,10 +2931,10 @@
         <v>335</v>
       </c>
       <c r="B72" t="s">
+        <v>117</v>
+      </c>
+      <c r="C72" t="s">
         <v>7</v>
-      </c>
-      <c r="C72" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
@@ -2942,10 +2942,10 @@
         <v>336</v>
       </c>
       <c r="B73" t="s">
+        <v>57</v>
+      </c>
+      <c r="C73" t="s">
         <v>118</v>
-      </c>
-      <c r="C73" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
@@ -2953,10 +2953,10 @@
         <v>271</v>
       </c>
       <c r="B74" t="s">
+        <v>120</v>
+      </c>
+      <c r="C74" t="s">
         <v>119</v>
-      </c>
-      <c r="C74" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
@@ -2964,10 +2964,10 @@
         <v>337</v>
       </c>
       <c r="B75" t="s">
+        <v>121</v>
+      </c>
+      <c r="C75" t="s">
         <v>77</v>
-      </c>
-      <c r="C75" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
@@ -2975,10 +2975,10 @@
         <v>338</v>
       </c>
       <c r="B76" t="s">
+        <v>123</v>
+      </c>
+      <c r="C76" t="s">
         <v>122</v>
-      </c>
-      <c r="C76" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
@@ -2986,10 +2986,10 @@
         <v>339</v>
       </c>
       <c r="B77" t="s">
+        <v>124</v>
+      </c>
+      <c r="C77" t="s">
         <v>119</v>
-      </c>
-      <c r="C77" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
@@ -2997,10 +2997,10 @@
         <v>340</v>
       </c>
       <c r="B78" t="s">
+        <v>78</v>
+      </c>
+      <c r="C78" t="s">
         <v>125</v>
-      </c>
-      <c r="C78" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
@@ -3008,10 +3008,10 @@
         <v>341</v>
       </c>
       <c r="B79" t="s">
+        <v>127</v>
+      </c>
+      <c r="C79" t="s">
         <v>126</v>
-      </c>
-      <c r="C79" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
@@ -3019,10 +3019,10 @@
         <v>342</v>
       </c>
       <c r="B80" t="s">
+        <v>129</v>
+      </c>
+      <c r="C80" t="s">
         <v>128</v>
-      </c>
-      <c r="C80" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
@@ -3030,10 +3030,10 @@
         <v>343</v>
       </c>
       <c r="B81" t="s">
+        <v>131</v>
+      </c>
+      <c r="C81" t="s">
         <v>130</v>
-      </c>
-      <c r="C81" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
@@ -3041,10 +3041,10 @@
         <v>344</v>
       </c>
       <c r="B82" t="s">
+        <v>133</v>
+      </c>
+      <c r="C82" t="s">
         <v>132</v>
-      </c>
-      <c r="C82" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
@@ -3052,10 +3052,10 @@
         <v>345</v>
       </c>
       <c r="B83" t="s">
+        <v>135</v>
+      </c>
+      <c r="C83" t="s">
         <v>134</v>
-      </c>
-      <c r="C83" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
@@ -3063,10 +3063,10 @@
         <v>277</v>
       </c>
       <c r="B84" t="s">
+        <v>59</v>
+      </c>
+      <c r="C84" t="s">
         <v>29</v>
-      </c>
-      <c r="C84" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
@@ -3074,10 +3074,10 @@
         <v>346</v>
       </c>
       <c r="B85" t="s">
+        <v>137</v>
+      </c>
+      <c r="C85" t="s">
         <v>136</v>
-      </c>
-      <c r="C85" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
@@ -3085,10 +3085,10 @@
         <v>347</v>
       </c>
       <c r="B86" t="s">
+        <v>139</v>
+      </c>
+      <c r="C86" t="s">
         <v>138</v>
-      </c>
-      <c r="C86" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
@@ -3096,10 +3096,10 @@
         <v>348</v>
       </c>
       <c r="B87" t="s">
+        <v>127</v>
+      </c>
+      <c r="C87" t="s">
         <v>110</v>
-      </c>
-      <c r="C87" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
@@ -3107,10 +3107,10 @@
         <v>349</v>
       </c>
       <c r="B88" t="s">
+        <v>140</v>
+      </c>
+      <c r="C88" t="s">
         <v>58</v>
-      </c>
-      <c r="C88" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
@@ -3118,10 +3118,10 @@
         <v>342</v>
       </c>
       <c r="B89" t="s">
+        <v>135</v>
+      </c>
+      <c r="C89" t="s">
         <v>138</v>
-      </c>
-      <c r="C89" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
@@ -3129,10 +3129,10 @@
         <v>350</v>
       </c>
       <c r="B90" t="s">
+        <v>141</v>
+      </c>
+      <c r="C90" t="s">
         <v>21</v>
-      </c>
-      <c r="C90" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
@@ -3140,10 +3140,10 @@
         <v>284</v>
       </c>
       <c r="B91" t="s">
+        <v>142</v>
+      </c>
+      <c r="C91" t="s">
         <v>58</v>
-      </c>
-      <c r="C91" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
@@ -3151,10 +3151,10 @@
         <v>351</v>
       </c>
       <c r="B92" t="s">
+        <v>143</v>
+      </c>
+      <c r="C92" t="s">
         <v>31</v>
-      </c>
-      <c r="C92" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
@@ -3162,10 +3162,10 @@
         <v>323</v>
       </c>
       <c r="B93" t="s">
+        <v>145</v>
+      </c>
+      <c r="C93" t="s">
         <v>144</v>
-      </c>
-      <c r="C93" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
@@ -3173,10 +3173,10 @@
         <v>352</v>
       </c>
       <c r="B94" t="s">
+        <v>147</v>
+      </c>
+      <c r="C94" t="s">
         <v>146</v>
-      </c>
-      <c r="C94" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
@@ -3184,10 +3184,10 @@
         <v>345</v>
       </c>
       <c r="B95" t="s">
+        <v>148</v>
+      </c>
+      <c r="C95" t="s">
         <v>23</v>
-      </c>
-      <c r="C95" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
@@ -3195,10 +3195,10 @@
         <v>326</v>
       </c>
       <c r="B96" t="s">
+        <v>150</v>
+      </c>
+      <c r="C96" t="s">
         <v>149</v>
-      </c>
-      <c r="C96" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
@@ -3206,10 +3206,10 @@
         <v>353</v>
       </c>
       <c r="B97" t="s">
+        <v>151</v>
+      </c>
+      <c r="C97" t="s">
         <v>7</v>
-      </c>
-      <c r="C97" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
@@ -3217,10 +3217,10 @@
         <v>322</v>
       </c>
       <c r="B98" t="s">
+        <v>153</v>
+      </c>
+      <c r="C98" t="s">
         <v>152</v>
-      </c>
-      <c r="C98" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
@@ -3228,10 +3228,10 @@
         <v>354</v>
       </c>
       <c r="B99" t="s">
+        <v>154</v>
+      </c>
+      <c r="C99" t="s">
         <v>17</v>
-      </c>
-      <c r="C99" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
@@ -3239,10 +3239,10 @@
         <v>355</v>
       </c>
       <c r="B100" t="s">
+        <v>156</v>
+      </c>
+      <c r="C100" t="s">
         <v>155</v>
-      </c>
-      <c r="C100" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
@@ -3250,10 +3250,10 @@
         <v>356</v>
       </c>
       <c r="B101" t="s">
+        <v>157</v>
+      </c>
+      <c r="C101" t="s">
         <v>21</v>
-      </c>
-      <c r="C101" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
@@ -3261,10 +3261,10 @@
         <v>357</v>
       </c>
       <c r="B102" t="s">
+        <v>158</v>
+      </c>
+      <c r="C102" t="s">
         <v>48</v>
-      </c>
-      <c r="C102" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
@@ -3272,10 +3272,10 @@
         <v>358</v>
       </c>
       <c r="B103" t="s">
+        <v>159</v>
+      </c>
+      <c r="C103" t="s">
         <v>81</v>
-      </c>
-      <c r="C103" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
@@ -3283,10 +3283,10 @@
         <v>359</v>
       </c>
       <c r="B104" t="s">
+        <v>39</v>
+      </c>
+      <c r="C104" t="s">
         <v>160</v>
-      </c>
-      <c r="C104" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
@@ -3294,10 +3294,10 @@
         <v>360</v>
       </c>
       <c r="B105" t="s">
+        <v>135</v>
+      </c>
+      <c r="C105" t="s">
         <v>161</v>
-      </c>
-      <c r="C105" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
@@ -3305,10 +3305,10 @@
         <v>293</v>
       </c>
       <c r="B106" t="s">
+        <v>89</v>
+      </c>
+      <c r="C106" t="s">
         <v>162</v>
-      </c>
-      <c r="C106" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
@@ -3316,10 +3316,10 @@
         <v>348</v>
       </c>
       <c r="B107" t="s">
+        <v>163</v>
+      </c>
+      <c r="C107" t="s">
         <v>119</v>
-      </c>
-      <c r="C107" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
@@ -3327,10 +3327,10 @@
         <v>361</v>
       </c>
       <c r="B108" t="s">
+        <v>164</v>
+      </c>
+      <c r="C108" t="s">
         <v>58</v>
-      </c>
-      <c r="C108" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
@@ -3338,10 +3338,10 @@
         <v>362</v>
       </c>
       <c r="B109" t="s">
+        <v>166</v>
+      </c>
+      <c r="C109" t="s">
         <v>165</v>
-      </c>
-      <c r="C109" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
@@ -3349,10 +3349,10 @@
         <v>363</v>
       </c>
       <c r="B110" t="s">
+        <v>20</v>
+      </c>
+      <c r="C110" t="s">
         <v>167</v>
-      </c>
-      <c r="C110" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
@@ -3360,10 +3360,10 @@
         <v>364</v>
       </c>
       <c r="B111" t="s">
+        <v>169</v>
+      </c>
+      <c r="C111" t="s">
         <v>168</v>
-      </c>
-      <c r="C111" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
@@ -3371,10 +3371,10 @@
         <v>305</v>
       </c>
       <c r="B112" t="s">
+        <v>170</v>
+      </c>
+      <c r="C112" t="s">
         <v>76</v>
-      </c>
-      <c r="C112" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
@@ -3382,10 +3382,10 @@
         <v>365</v>
       </c>
       <c r="B113" t="s">
+        <v>93</v>
+      </c>
+      <c r="C113" t="s">
         <v>52</v>
-      </c>
-      <c r="C113" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
@@ -3393,10 +3393,10 @@
         <v>366</v>
       </c>
       <c r="B114" t="s">
+        <v>123</v>
+      </c>
+      <c r="C114" t="s">
         <v>171</v>
-      </c>
-      <c r="C114" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
@@ -3404,10 +3404,10 @@
         <v>367</v>
       </c>
       <c r="B115" t="s">
+        <v>173</v>
+      </c>
+      <c r="C115" t="s">
         <v>172</v>
-      </c>
-      <c r="C115" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
@@ -3415,10 +3415,10 @@
         <v>368</v>
       </c>
       <c r="B116" t="s">
+        <v>175</v>
+      </c>
+      <c r="C116" t="s">
         <v>174</v>
-      </c>
-      <c r="C116" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
@@ -3426,10 +3426,10 @@
         <v>369</v>
       </c>
       <c r="B117" t="s">
+        <v>154</v>
+      </c>
+      <c r="C117" t="s">
         <v>176</v>
-      </c>
-      <c r="C117" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
@@ -3437,10 +3437,10 @@
         <v>370</v>
       </c>
       <c r="B118" t="s">
+        <v>178</v>
+      </c>
+      <c r="C118" t="s">
         <v>177</v>
-      </c>
-      <c r="C118" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
@@ -3448,10 +3448,10 @@
         <v>371</v>
       </c>
       <c r="B119" t="s">
+        <v>180</v>
+      </c>
+      <c r="C119" t="s">
         <v>179</v>
-      </c>
-      <c r="C119" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
@@ -3459,10 +3459,10 @@
         <v>372</v>
       </c>
       <c r="B120" t="s">
+        <v>182</v>
+      </c>
+      <c r="C120" t="s">
         <v>181</v>
-      </c>
-      <c r="C120" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
@@ -3470,10 +3470,10 @@
         <v>373</v>
       </c>
       <c r="B121" t="s">
+        <v>184</v>
+      </c>
+      <c r="C121" t="s">
         <v>183</v>
-      </c>
-      <c r="C121" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
@@ -3481,10 +3481,10 @@
         <v>357</v>
       </c>
       <c r="B122" t="s">
+        <v>185</v>
+      </c>
+      <c r="C122" t="s">
         <v>165</v>
-      </c>
-      <c r="C122" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
@@ -3492,10 +3492,10 @@
         <v>374</v>
       </c>
       <c r="B123" t="s">
+        <v>141</v>
+      </c>
+      <c r="C123" t="s">
         <v>186</v>
-      </c>
-      <c r="C123" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
@@ -3503,10 +3503,10 @@
         <v>375</v>
       </c>
       <c r="B124" t="s">
+        <v>188</v>
+      </c>
+      <c r="C124" t="s">
         <v>187</v>
-      </c>
-      <c r="C124" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
@@ -3514,10 +3514,10 @@
         <v>356</v>
       </c>
       <c r="B125" t="s">
+        <v>190</v>
+      </c>
+      <c r="C125" t="s">
         <v>189</v>
-      </c>
-      <c r="C125" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
@@ -3525,10 +3525,10 @@
         <v>376</v>
       </c>
       <c r="B126" t="s">
+        <v>191</v>
+      </c>
+      <c r="C126" t="s">
         <v>176</v>
-      </c>
-      <c r="C126" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
@@ -3536,10 +3536,10 @@
         <v>377</v>
       </c>
       <c r="B127" t="s">
+        <v>193</v>
+      </c>
+      <c r="C127" t="s">
         <v>192</v>
-      </c>
-      <c r="C127" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
@@ -3547,10 +3547,10 @@
         <v>314</v>
       </c>
       <c r="B128" t="s">
+        <v>195</v>
+      </c>
+      <c r="C128" t="s">
         <v>194</v>
-      </c>
-      <c r="C128" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
@@ -3558,10 +3558,10 @@
         <v>271</v>
       </c>
       <c r="B129" t="s">
+        <v>197</v>
+      </c>
+      <c r="C129" t="s">
         <v>196</v>
-      </c>
-      <c r="C129" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
@@ -3569,10 +3569,10 @@
         <v>378</v>
       </c>
       <c r="B130" t="s">
+        <v>49</v>
+      </c>
+      <c r="C130" t="s">
         <v>79</v>
-      </c>
-      <c r="C130" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
@@ -3580,10 +3580,10 @@
         <v>379</v>
       </c>
       <c r="B131" t="s">
+        <v>199</v>
+      </c>
+      <c r="C131" t="s">
         <v>198</v>
-      </c>
-      <c r="C131" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
@@ -3591,10 +3591,10 @@
         <v>380</v>
       </c>
       <c r="B132" t="s">
+        <v>201</v>
+      </c>
+      <c r="C132" t="s">
         <v>200</v>
-      </c>
-      <c r="C132" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
@@ -3602,10 +3602,10 @@
         <v>381</v>
       </c>
       <c r="B133" t="s">
+        <v>203</v>
+      </c>
+      <c r="C133" t="s">
         <v>202</v>
-      </c>
-      <c r="C133" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
@@ -3613,10 +3613,10 @@
         <v>372</v>
       </c>
       <c r="B134" t="s">
+        <v>205</v>
+      </c>
+      <c r="C134" t="s">
         <v>204</v>
-      </c>
-      <c r="C134" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
@@ -3624,10 +3624,10 @@
         <v>382</v>
       </c>
       <c r="B135" t="s">
+        <v>207</v>
+      </c>
+      <c r="C135" t="s">
         <v>206</v>
-      </c>
-      <c r="C135" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
@@ -3635,10 +3635,10 @@
         <v>383</v>
       </c>
       <c r="B136" t="s">
+        <v>209</v>
+      </c>
+      <c r="C136" t="s">
         <v>208</v>
-      </c>
-      <c r="C136" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
@@ -3646,10 +3646,10 @@
         <v>308</v>
       </c>
       <c r="B137" t="s">
+        <v>211</v>
+      </c>
+      <c r="C137" t="s">
         <v>210</v>
-      </c>
-      <c r="C137" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
@@ -3657,10 +3657,10 @@
         <v>384</v>
       </c>
       <c r="B138" t="s">
+        <v>121</v>
+      </c>
+      <c r="C138" t="s">
         <v>212</v>
-      </c>
-      <c r="C138" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
@@ -3668,10 +3668,10 @@
         <v>385</v>
       </c>
       <c r="B139" t="s">
+        <v>59</v>
+      </c>
+      <c r="C139" t="s">
         <v>213</v>
-      </c>
-      <c r="C139" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
@@ -3679,10 +3679,10 @@
         <v>386</v>
       </c>
       <c r="B140" t="s">
+        <v>215</v>
+      </c>
+      <c r="C140" t="s">
         <v>214</v>
-      </c>
-      <c r="C140" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
@@ -3690,10 +3690,10 @@
         <v>387</v>
       </c>
       <c r="B141" t="s">
+        <v>217</v>
+      </c>
+      <c r="C141" t="s">
         <v>216</v>
-      </c>
-      <c r="C141" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
@@ -3701,10 +3701,10 @@
         <v>388</v>
       </c>
       <c r="B142" t="s">
+        <v>218</v>
+      </c>
+      <c r="C142" t="s">
         <v>136</v>
-      </c>
-      <c r="C142" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
@@ -3712,10 +3712,10 @@
         <v>389</v>
       </c>
       <c r="B143" t="s">
+        <v>220</v>
+      </c>
+      <c r="C143" t="s">
         <v>219</v>
-      </c>
-      <c r="C143" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
@@ -3723,10 +3723,10 @@
         <v>390</v>
       </c>
       <c r="B144" t="s">
+        <v>222</v>
+      </c>
+      <c r="C144" t="s">
         <v>221</v>
-      </c>
-      <c r="C144" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
@@ -3734,10 +3734,10 @@
         <v>391</v>
       </c>
       <c r="B145" t="s">
+        <v>224</v>
+      </c>
+      <c r="C145" t="s">
         <v>223</v>
-      </c>
-      <c r="C145" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
@@ -3745,10 +3745,10 @@
         <v>392</v>
       </c>
       <c r="B146" t="s">
+        <v>226</v>
+      </c>
+      <c r="C146" t="s">
         <v>225</v>
-      </c>
-      <c r="C146" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
@@ -3756,10 +3756,10 @@
         <v>393</v>
       </c>
       <c r="B147" t="s">
+        <v>106</v>
+      </c>
+      <c r="C147" t="s">
         <v>227</v>
-      </c>
-      <c r="C147" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
@@ -3767,10 +3767,10 @@
         <v>394</v>
       </c>
       <c r="B148" t="s">
+        <v>229</v>
+      </c>
+      <c r="C148" t="s">
         <v>228</v>
-      </c>
-      <c r="C148" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
@@ -3778,10 +3778,10 @@
         <v>321</v>
       </c>
       <c r="B149" t="s">
+        <v>88</v>
+      </c>
+      <c r="C149" t="s">
         <v>230</v>
-      </c>
-      <c r="C149" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
@@ -3789,10 +3789,10 @@
         <v>395</v>
       </c>
       <c r="B150" t="s">
+        <v>232</v>
+      </c>
+      <c r="C150" t="s">
         <v>231</v>
-      </c>
-      <c r="C150" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
@@ -3800,10 +3800,10 @@
         <v>396</v>
       </c>
       <c r="B151" t="s">
+        <v>234</v>
+      </c>
+      <c r="C151" t="s">
         <v>233</v>
-      </c>
-      <c r="C151" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
@@ -3811,10 +3811,10 @@
         <v>397</v>
       </c>
       <c r="B152" t="s">
+        <v>235</v>
+      </c>
+      <c r="C152" t="s">
         <v>56</v>
-      </c>
-      <c r="C152" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
@@ -3822,10 +3822,10 @@
         <v>368</v>
       </c>
       <c r="B153" t="s">
+        <v>135</v>
+      </c>
+      <c r="C153" t="s">
         <v>236</v>
-      </c>
-      <c r="C153" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
@@ -3833,10 +3833,10 @@
         <v>398</v>
       </c>
       <c r="B154" t="s">
+        <v>150</v>
+      </c>
+      <c r="C154" t="s">
         <v>77</v>
-      </c>
-      <c r="C154" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
@@ -3844,10 +3844,10 @@
         <v>399</v>
       </c>
       <c r="B155" t="s">
+        <v>238</v>
+      </c>
+      <c r="C155" t="s">
         <v>237</v>
-      </c>
-      <c r="C155" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
@@ -3855,10 +3855,10 @@
         <v>360</v>
       </c>
       <c r="B156" t="s">
+        <v>51</v>
+      </c>
+      <c r="C156" t="s">
         <v>179</v>
-      </c>
-      <c r="C156" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
@@ -3866,10 +3866,10 @@
         <v>400</v>
       </c>
       <c r="B157" t="s">
+        <v>239</v>
+      </c>
+      <c r="C157" t="s">
         <v>231</v>
-      </c>
-      <c r="C157" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
@@ -3877,10 +3877,10 @@
         <v>401</v>
       </c>
       <c r="B158" t="s">
+        <v>20</v>
+      </c>
+      <c r="C158" t="s">
         <v>212</v>
-      </c>
-      <c r="C158" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
@@ -3888,10 +3888,10 @@
         <v>402</v>
       </c>
       <c r="B159" t="s">
+        <v>241</v>
+      </c>
+      <c r="C159" t="s">
         <v>240</v>
-      </c>
-      <c r="C159" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
@@ -3899,10 +3899,10 @@
         <v>403</v>
       </c>
       <c r="B160" t="s">
+        <v>242</v>
+      </c>
+      <c r="C160" t="s">
         <v>219</v>
-      </c>
-      <c r="C160" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
@@ -3910,10 +3910,10 @@
         <v>376</v>
       </c>
       <c r="B161" t="s">
+        <v>243</v>
+      </c>
+      <c r="C161" t="s">
         <v>48</v>
-      </c>
-      <c r="C161" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
@@ -3921,10 +3921,10 @@
         <v>404</v>
       </c>
       <c r="B162" t="s">
+        <v>245</v>
+      </c>
+      <c r="C162" t="s">
         <v>244</v>
-      </c>
-      <c r="C162" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
@@ -3932,10 +3932,10 @@
         <v>347</v>
       </c>
       <c r="B163" t="s">
+        <v>141</v>
+      </c>
+      <c r="C163" t="s">
         <v>38</v>
-      </c>
-      <c r="C163" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
@@ -3943,10 +3943,10 @@
         <v>405</v>
       </c>
       <c r="B164" t="s">
+        <v>247</v>
+      </c>
+      <c r="C164" t="s">
         <v>246</v>
-      </c>
-      <c r="C164" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
@@ -3954,10 +3954,10 @@
         <v>321</v>
       </c>
       <c r="B165" t="s">
+        <v>249</v>
+      </c>
+      <c r="C165" t="s">
         <v>248</v>
-      </c>
-      <c r="C165" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
@@ -3965,10 +3965,10 @@
         <v>406</v>
       </c>
       <c r="B166" t="s">
+        <v>207</v>
+      </c>
+      <c r="C166" t="s">
         <v>200</v>
-      </c>
-      <c r="C166" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
@@ -3976,10 +3976,10 @@
         <v>407</v>
       </c>
       <c r="B167" t="s">
+        <v>251</v>
+      </c>
+      <c r="C167" t="s">
         <v>250</v>
-      </c>
-      <c r="C167" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
@@ -3987,10 +3987,10 @@
         <v>408</v>
       </c>
       <c r="B168" t="s">
+        <v>252</v>
+      </c>
+      <c r="C168" t="s">
         <v>101</v>
-      </c>
-      <c r="C168" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
@@ -3998,10 +3998,10 @@
         <v>409</v>
       </c>
       <c r="B169" t="s">
+        <v>253</v>
+      </c>
+      <c r="C169" t="s">
         <v>165</v>
-      </c>
-      <c r="C169" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
@@ -4009,10 +4009,10 @@
         <v>410</v>
       </c>
       <c r="B170" t="s">
+        <v>135</v>
+      </c>
+      <c r="C170" t="s">
         <v>236</v>
-      </c>
-      <c r="C170" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
@@ -4020,10 +4020,10 @@
         <v>411</v>
       </c>
       <c r="B171" t="s">
+        <v>254</v>
+      </c>
+      <c r="C171" t="s">
         <v>31</v>
-      </c>
-      <c r="C171" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
@@ -4031,10 +4031,10 @@
         <v>412</v>
       </c>
       <c r="B172" t="s">
+        <v>256</v>
+      </c>
+      <c r="C172" t="s">
         <v>255</v>
-      </c>
-      <c r="C172" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
@@ -4042,10 +4042,10 @@
         <v>413</v>
       </c>
       <c r="B173" t="s">
+        <v>257</v>
+      </c>
+      <c r="C173" t="s">
         <v>138</v>
-      </c>
-      <c r="C173" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
@@ -4053,10 +4053,10 @@
         <v>400</v>
       </c>
       <c r="B174" t="s">
+        <v>118</v>
+      </c>
+      <c r="C174" t="s">
         <v>258</v>
-      </c>
-      <c r="C174" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
@@ -4064,10 +4064,10 @@
         <v>414</v>
       </c>
       <c r="B175" t="s">
+        <v>259</v>
+      </c>
+      <c r="C175" t="s">
         <v>225</v>
-      </c>
-      <c r="C175" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
@@ -4075,10 +4075,10 @@
         <v>281</v>
       </c>
       <c r="B176" t="s">
+        <v>261</v>
+      </c>
+      <c r="C176" t="s">
         <v>260</v>
-      </c>
-      <c r="C176" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
@@ -4086,10 +4086,10 @@
         <v>415</v>
       </c>
       <c r="B177" t="s">
+        <v>218</v>
+      </c>
+      <c r="C177" t="s">
         <v>221</v>
-      </c>
-      <c r="C177" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
@@ -4097,10 +4097,10 @@
         <v>304</v>
       </c>
       <c r="B178" t="s">
+        <v>12</v>
+      </c>
+      <c r="C178" t="s">
         <v>262</v>
-      </c>
-      <c r="C178" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
@@ -4108,10 +4108,10 @@
         <v>416</v>
       </c>
       <c r="B179" t="s">
+        <v>263</v>
+      </c>
+      <c r="C179" t="s">
         <v>262</v>
-      </c>
-      <c r="C179" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
@@ -4119,10 +4119,10 @@
         <v>417</v>
       </c>
       <c r="B180" t="s">
+        <v>264</v>
+      </c>
+      <c r="C180" t="s">
         <v>48</v>
-      </c>
-      <c r="C180" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
@@ -4130,10 +4130,10 @@
         <v>287</v>
       </c>
       <c r="B181" t="s">
+        <v>266</v>
+      </c>
+      <c r="C181" t="s">
         <v>265</v>
-      </c>
-      <c r="C181" t="s">
-        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>